<commit_message>
Sun Apr 26 14:00:00 IST 2020
</commit_message>
<xml_diff>
--- a/output/reports/01-Network-Audit.xlsx
+++ b/output/reports/01-Network-Audit.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>TCL NETWORK ASSESSMENT - WAN NETWORK DEVICE ACCESS EXAMINATION MODULE</t>
   </si>
@@ -43,16 +43,40 @@
     <t>CPU-UTILS</t>
   </si>
   <si>
-    <t>192.168.0.105</t>
-  </si>
-  <si>
-    <t>gimec-lab-1</t>
+    <t>192.168.0.106</t>
+  </si>
+  <si>
+    <t>lab-3725</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>5</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>192.168.0.107</t>
+  </si>
+  <si>
+    <t>lab-3660</t>
+  </si>
+  <si>
+    <t>192.168.0.108</t>
+  </si>
+  <si>
+    <t>lab-3640</t>
+  </si>
+  <si>
+    <t>192.168.0.109</t>
+  </si>
+  <si>
+    <t>lab-3745</t>
+  </si>
+  <si>
+    <t>192.168.0.110</t>
+  </si>
+  <si>
+    <t>lab-2691</t>
   </si>
 </sst>
 </file>
@@ -429,7 +453,7 @@
   <sheetPr>
     <tabColor rgb="FF808080"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -500,6 +524,98 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A4:G4"/>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Mon Apr 27 14:36:49 IST 2020
</commit_message>
<xml_diff>
--- a/output/reports/01-Network-Audit.xlsx
+++ b/output/reports/01-Network-Audit.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>TCL NETWORK ASSESSMENT - WAN NETWORK DEVICE ACCESS EXAMINATION MODULE</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>lab-3660</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
   <si>
     <t>192.168.0.108</t>
@@ -541,10 +547,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -552,22 +558,22 @@
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -575,10 +581,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>10</v>
@@ -590,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -598,10 +604,10 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>10</v>

</xml_diff>